<commit_message>
Messergebnisse der Verstärkerschaltung (Temp Sensor)
</commit_message>
<xml_diff>
--- a/hardware/Verstaerker/Amplifier.xlsx
+++ b/hardware/Verstaerker/Amplifier.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Messwerte Tempsensor Verstärker</t>
   </si>
@@ -38,13 +38,30 @@
   <si>
     <t>Formel (Ua*-0,5)+3,15</t>
   </si>
+  <si>
+    <t>Ub in mV</t>
+  </si>
+  <si>
+    <t>Ua in mV</t>
+  </si>
+  <si>
+    <t>unverstärkt</t>
+  </si>
+  <si>
+    <t>verstärkt</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000\ &quot;V&quot;"/>
+    <numFmt numFmtId="165" formatCode="0\ &quot;mV&quot;"/>
+    <numFmt numFmtId="167" formatCode="0.00\ &quot;°C&quot;"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -127,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -136,6 +153,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -185,11 +206,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$B$4</c:f>
+              <c:f>Tabelle1!$C$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ub</c:v>
+                  <c:v>Ub in mV</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -229,33 +250,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$5:$B$12</c:f>
+              <c:f>Tabelle1!$C$5:$C$12</c:f>
               <c:numCache>
-                <c:formatCode>0.000\ "V"</c:formatCode>
+                <c:formatCode>0\ "mV"</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.90300000000000002</c:v>
+                  <c:v>903</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1080000000000001</c:v>
+                  <c:v>1108</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.004</c:v>
+                  <c:v>1004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2</c:v>
+                  <c:v>1200</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.401</c:v>
+                  <c:v>1401</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.603</c:v>
+                  <c:v>1603</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.7</c:v>
+                  <c:v>1700</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.8009999999999999</c:v>
+                  <c:v>1801</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -267,7 +288,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$D$4</c:f>
+              <c:f>Tabelle1!$F$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -311,33 +332,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$D$5:$D$12</c:f>
+              <c:f>Tabelle1!$G$5:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>0.000\ "V"</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.90850000000000009</c:v>
+                  <c:v>908.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1225000000000001</c:v>
+                  <c:v>1122.5000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0329999999999999</c:v>
+                  <c:v>1033</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.238</c:v>
+                  <c:v>1238</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.45</c:v>
+                  <c:v>1450</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6639999999999999</c:v>
+                  <c:v>1664</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.766</c:v>
+                  <c:v>1766</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.8739999999999999</c:v>
+                  <c:v>1874</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -349,7 +370,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$C$4</c:f>
+              <c:f>Tabelle1!$D$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -393,33 +414,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$C$5:$C$12</c:f>
+              <c:f>Tabelle1!$E$5:$E$12</c:f>
               <c:numCache>
-                <c:formatCode>0.000\ "V"</c:formatCode>
+                <c:formatCode>0\ "mV"</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>4.4829999999999997</c:v>
+                  <c:v>4483</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.0549999999999997</c:v>
+                  <c:v>4054.9999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.234</c:v>
+                  <c:v>4234</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.8239999999999998</c:v>
+                  <c:v>3824</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.4</c:v>
+                  <c:v>3400</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.972</c:v>
+                  <c:v>2972</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.7679999999999998</c:v>
+                  <c:v>2768</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.552</c:v>
+                  <c:v>2552</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -436,11 +457,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="94898432"/>
-        <c:axId val="94900224"/>
+        <c:axId val="98700288"/>
+        <c:axId val="98702080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="94898432"/>
+        <c:axId val="98700288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -450,7 +471,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94900224"/>
+        <c:crossAx val="98702080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -458,7 +479,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94900224"/>
+        <c:axId val="98702080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.8"/>
@@ -466,11 +487,11 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.000\ &quot;V&quot;" sourceLinked="1"/>
+        <c:numFmt formatCode="0\ &quot;mV&quot;" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94898432"/>
+        <c:crossAx val="98700288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -501,20 +522,401 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$C$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>unverstärkt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$B$18:$B$38</c:f>
+              <c:numCache>
+                <c:formatCode>0\ "mV"</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>870</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>880</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>890</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>910</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>920</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>930</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>940</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>960</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>970</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>990</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$C$18:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.00\ "°C"</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>-3.41</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.4300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.48</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.58</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.55</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.54</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.58</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.56</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.5299999999999994</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10.51</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$D$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>verstärkt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$B$18:$B$38</c:f>
+              <c:numCache>
+                <c:formatCode>0\ "mV"</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>870</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>880</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>890</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>910</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>920</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>930</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>940</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>960</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>970</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>990</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$D$18:$D$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.00\ "°C"</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>-4.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.33</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.91</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.78</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.81</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.91</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.9499999999999993</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10.17</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11.33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="96320128"/>
+        <c:axId val="96326016"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="96320128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0\ &quot;mV&quot;" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="96326016"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="96326016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00\ &quot;°C&quot;" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="96320128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -528,6 +930,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>309561</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>185736</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>161924</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -823,137 +1255,569 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D12"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
         <v>0.90300000000000002</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="8">
+        <f>B5*1000</f>
+        <v>903</v>
+      </c>
+      <c r="D5" s="2">
         <v>4.4829999999999997</v>
       </c>
-      <c r="D5" s="2">
-        <f>(C5*-0.5)+3.15</f>
+      <c r="E5" s="8">
+        <f>D5*1000</f>
+        <v>4483</v>
+      </c>
+      <c r="F5" s="2">
+        <f>(D5*-0.5)+3.15</f>
         <v>0.90850000000000009</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5" s="2">
+        <f>(E5*-0.5)+3150</f>
+        <v>908.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="5">
         <v>1.1080000000000001</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="8">
+        <f t="shared" ref="C6:E12" si="0">B6*1000</f>
+        <v>1108</v>
+      </c>
+      <c r="D6" s="2">
         <v>4.0549999999999997</v>
       </c>
-      <c r="D6" s="2">
-        <f t="shared" ref="D6:D12" si="0">(C6*-0.5)+3.15</f>
+      <c r="E6" s="8">
+        <f t="shared" si="0"/>
+        <v>4054.9999999999995</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" ref="F6:F12" si="1">(D6*-0.5)+3.15</f>
         <v>1.1225000000000001</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" s="2">
+        <f t="shared" ref="G6:G12" si="2">(E6*-0.5)+3150</f>
+        <v>1122.5000000000002</v>
+      </c>
+      <c r="H6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
         <v>1.004</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="8">
+        <f t="shared" si="0"/>
+        <v>1004</v>
+      </c>
+      <c r="D7" s="2">
         <v>4.234</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="8">
         <f t="shared" si="0"/>
+        <v>4234</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="1"/>
         <v>1.0329999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G7" s="2">
+        <f t="shared" si="2"/>
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
         <v>1.2</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="8">
+        <f t="shared" si="0"/>
+        <v>1200</v>
+      </c>
+      <c r="D8" s="2">
         <v>3.8239999999999998</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="8">
         <f t="shared" si="0"/>
+        <v>3824</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="1"/>
         <v>1.238</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G8" s="2">
+        <f t="shared" si="2"/>
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>1.401</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="8">
+        <f t="shared" si="0"/>
+        <v>1401</v>
+      </c>
+      <c r="D9" s="2">
         <v>3.4</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="8">
         <f t="shared" si="0"/>
+        <v>3400</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="1"/>
         <v>1.45</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9" s="2">
+        <f t="shared" si="2"/>
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>1.603</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="8">
+        <f t="shared" si="0"/>
+        <v>1603</v>
+      </c>
+      <c r="D10" s="2">
         <v>2.972</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E10" s="8">
         <f t="shared" si="0"/>
+        <v>2972</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="1"/>
         <v>1.6639999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G10" s="2">
+        <f t="shared" si="2"/>
+        <v>1664</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
         <v>1.7</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="8">
+        <f t="shared" si="0"/>
+        <v>1700</v>
+      </c>
+      <c r="D11" s="2">
         <v>2.7679999999999998</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E11" s="8">
         <f t="shared" si="0"/>
+        <v>2768</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="1"/>
         <v>1.766</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G11" s="2">
+        <f t="shared" si="2"/>
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
         <v>1.8009999999999999</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="8">
+        <f t="shared" si="0"/>
+        <v>1801</v>
+      </c>
+      <c r="D12" s="2">
         <v>2.552</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E12" s="8">
         <f t="shared" si="0"/>
+        <v>2552</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="1"/>
         <v>1.8739999999999999</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="2"/>
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="9">
+        <v>850</v>
+      </c>
+      <c r="C18" s="10">
+        <v>-3.41</v>
+      </c>
+      <c r="D18" s="10">
+        <v>-4.2</v>
+      </c>
+      <c r="E18" s="11">
+        <f>C18-D18</f>
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="9">
+        <v>860</v>
+      </c>
+      <c r="C19" s="10">
+        <v>-2.4300000000000002</v>
+      </c>
+      <c r="D19" s="10">
+        <v>-3.3</v>
+      </c>
+      <c r="E19" s="11">
+        <f t="shared" ref="E19:E38" si="3">C19-D19</f>
+        <v>0.86999999999999966</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="9">
+        <v>870</v>
+      </c>
+      <c r="C20" s="10">
+        <v>-1.45</v>
+      </c>
+      <c r="D20" s="10">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="E20" s="11">
+        <f t="shared" si="3"/>
+        <v>0.75000000000000022</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="9">
+        <v>880</v>
+      </c>
+      <c r="C21" s="10">
+        <v>-0.35</v>
+      </c>
+      <c r="D21" s="10">
+        <v>-1.3</v>
+      </c>
+      <c r="E21" s="11">
+        <f t="shared" si="3"/>
+        <v>0.95000000000000007</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="9">
+        <v>890</v>
+      </c>
+      <c r="C22" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="10">
+        <v>-0.33</v>
+      </c>
+      <c r="E22" s="11">
+        <f t="shared" si="3"/>
+        <v>0.83000000000000007</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="9">
+        <v>900</v>
+      </c>
+      <c r="C23" s="10">
+        <v>1.48</v>
+      </c>
+      <c r="D23" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="E23" s="11">
+        <f t="shared" si="3"/>
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="9">
+        <v>910</v>
+      </c>
+      <c r="C24" s="10">
+        <v>2.58</v>
+      </c>
+      <c r="D24" s="10">
+        <v>1.75</v>
+      </c>
+      <c r="E24" s="11">
+        <f t="shared" si="3"/>
+        <v>0.83000000000000007</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="9">
+        <v>920</v>
+      </c>
+      <c r="C25" s="10">
+        <v>3.55</v>
+      </c>
+      <c r="D25" s="10">
+        <v>2.91</v>
+      </c>
+      <c r="E25" s="11">
+        <f t="shared" si="3"/>
+        <v>0.63999999999999968</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="9">
+        <v>930</v>
+      </c>
+      <c r="C26" s="10">
+        <v>4.54</v>
+      </c>
+      <c r="D26" s="10">
+        <v>3.7</v>
+      </c>
+      <c r="E26" s="11">
+        <f t="shared" si="3"/>
+        <v>0.83999999999999986</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="9">
+        <v>940</v>
+      </c>
+      <c r="C27" s="10">
+        <v>5.5</v>
+      </c>
+      <c r="D27" s="10">
+        <v>4.8</v>
+      </c>
+      <c r="E27" s="11">
+        <f t="shared" si="3"/>
+        <v>0.70000000000000018</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="9">
+        <v>950</v>
+      </c>
+      <c r="C28" s="10">
+        <v>6.6</v>
+      </c>
+      <c r="D28" s="10">
+        <v>5.78</v>
+      </c>
+      <c r="E28" s="11">
+        <f t="shared" si="3"/>
+        <v>0.8199999999999994</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="9">
+        <v>960</v>
+      </c>
+      <c r="C29" s="10">
+        <v>7.58</v>
+      </c>
+      <c r="D29" s="10">
+        <v>6.81</v>
+      </c>
+      <c r="E29" s="11">
+        <f t="shared" si="3"/>
+        <v>0.77000000000000046</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="9">
+        <v>970</v>
+      </c>
+      <c r="C30" s="10">
+        <v>8.56</v>
+      </c>
+      <c r="D30" s="10">
+        <v>7.91</v>
+      </c>
+      <c r="E30" s="11">
+        <f t="shared" si="3"/>
+        <v>0.65000000000000036</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="9">
+        <v>980</v>
+      </c>
+      <c r="C31" s="10">
+        <v>9.5299999999999994</v>
+      </c>
+      <c r="D31" s="10">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="E31" s="11">
+        <f t="shared" si="3"/>
+        <v>0.58000000000000007</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="9">
+        <v>990</v>
+      </c>
+      <c r="C32" s="10">
+        <v>10.51</v>
+      </c>
+      <c r="D32" s="10">
+        <v>10.17</v>
+      </c>
+      <c r="E32" s="11">
+        <f t="shared" si="3"/>
+        <v>0.33999999999999986</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="9">
+        <v>1000</v>
+      </c>
+      <c r="C33" s="10">
+        <v>11.98</v>
+      </c>
+      <c r="D33" s="10">
+        <v>11.33</v>
+      </c>
+      <c r="E33" s="11">
+        <f t="shared" si="3"/>
+        <v>0.65000000000000036</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="9">
+        <v>1100</v>
+      </c>
+      <c r="C34" s="10">
+        <v>21.86</v>
+      </c>
+      <c r="D34" s="10">
+        <v>21.89</v>
+      </c>
+      <c r="E34" s="11">
+        <f t="shared" si="3"/>
+        <v>-3.0000000000001137E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="9">
+        <v>1200</v>
+      </c>
+      <c r="C35" s="10">
+        <v>32.119999999999997</v>
+      </c>
+      <c r="D35" s="10">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="E35" s="11">
+        <f t="shared" si="3"/>
+        <v>-8.00000000000054E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="9">
+        <v>1300</v>
+      </c>
+      <c r="C36" s="10">
+        <v>42</v>
+      </c>
+      <c r="D36" s="10">
+        <v>42.8</v>
+      </c>
+      <c r="E36" s="11">
+        <f t="shared" si="3"/>
+        <v>-0.79999999999999716</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="9">
+        <v>1400</v>
+      </c>
+      <c r="C37" s="10">
+        <v>52.89</v>
+      </c>
+      <c r="D37" s="10">
+        <v>52.9</v>
+      </c>
+      <c r="E37" s="11">
+        <f t="shared" si="3"/>
+        <v>-9.9999999999980105E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="9">
+        <v>1500</v>
+      </c>
+      <c r="C38" s="10">
+        <v>62.15</v>
+      </c>
+      <c r="D38" s="10">
+        <v>64.13</v>
+      </c>
+      <c r="E38" s="11">
+        <f t="shared" si="3"/>
+        <v>-1.9799999999999969</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Formula for lm35 with ampifier
</commit_message>
<xml_diff>
--- a/hardware/Verstaerker/Amplifier.xlsx
+++ b/hardware/Verstaerker/Amplifier.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Messwerte Tempsensor Verstärker</t>
   </si>
@@ -53,6 +53,9 @@
   <si>
     <t>delta</t>
   </si>
+  <si>
+    <t xml:space="preserve"> (909mV offset)</t>
+  </si>
 </sst>
 </file>
 
@@ -61,9 +64,9 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000\ &quot;V&quot;"/>
     <numFmt numFmtId="165" formatCode="0\ &quot;mV&quot;"/>
-    <numFmt numFmtId="167" formatCode="0.00\ &quot;°C&quot;"/>
+    <numFmt numFmtId="166" formatCode="0.00\ &quot;°C&quot;"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +92,13 @@
     <font>
       <i/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -144,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -155,8 +165,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -334,7 +345,7 @@
             <c:numRef>
               <c:f>Tabelle1!$G$5:$G$12</c:f>
               <c:numCache>
-                <c:formatCode>0.000\ "V"</c:formatCode>
+                <c:formatCode>0\ "mV"</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>908.5</c:v>
@@ -457,11 +468,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="98700288"/>
-        <c:axId val="98702080"/>
+        <c:axId val="100412416"/>
+        <c:axId val="100414208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98700288"/>
+        <c:axId val="100412416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -471,7 +482,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98702080"/>
+        <c:crossAx val="100414208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -479,7 +490,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98702080"/>
+        <c:axId val="100414208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.8"/>
@@ -491,7 +502,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98700288"/>
+        <c:crossAx val="100412416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -848,11 +859,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="96320128"/>
-        <c:axId val="96326016"/>
+        <c:axId val="100448128"/>
+        <c:axId val="100449664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96320128"/>
+        <c:axId val="100448128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -862,7 +873,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96326016"/>
+        <c:crossAx val="100449664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -870,7 +881,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96326016"/>
+        <c:axId val="100449664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -881,7 +892,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96320128"/>
+        <c:crossAx val="100448128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1257,11 +1268,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -1274,7 +1288,9 @@
       </c>
     </row>
     <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="A4" s="12" t="s">
+        <v>12</v>
+      </c>
       <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
@@ -1312,7 +1328,7 @@
         <f>(D5*-0.5)+3.15</f>
         <v>0.90850000000000009</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="9">
         <f>(E5*-0.5)+3150</f>
         <v>908.5</v>
       </c>
@@ -1339,7 +1355,7 @@
         <f t="shared" ref="F6:F12" si="1">(D6*-0.5)+3.15</f>
         <v>1.1225000000000001</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="9">
         <f t="shared" ref="G6:G12" si="2">(E6*-0.5)+3150</f>
         <v>1122.5000000000002</v>
       </c>
@@ -1366,7 +1382,7 @@
         <f t="shared" si="1"/>
         <v>1.0329999999999999</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="9">
         <f t="shared" si="2"/>
         <v>1033</v>
       </c>
@@ -1390,7 +1406,7 @@
         <f t="shared" si="1"/>
         <v>1.238</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="9">
         <f t="shared" si="2"/>
         <v>1238</v>
       </c>
@@ -1414,7 +1430,7 @@
         <f t="shared" si="1"/>
         <v>1.45</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="9">
         <f t="shared" si="2"/>
         <v>1450</v>
       </c>
@@ -1438,7 +1454,7 @@
         <f t="shared" si="1"/>
         <v>1.6639999999999999</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="9">
         <f t="shared" si="2"/>
         <v>1664</v>
       </c>
@@ -1462,7 +1478,7 @@
         <f t="shared" si="1"/>
         <v>1.766</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="9">
         <f t="shared" si="2"/>
         <v>1766</v>
       </c>
@@ -1486,7 +1502,7 @@
         <f t="shared" si="1"/>
         <v>1.8739999999999999</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="9">
         <f t="shared" si="2"/>
         <v>1874</v>
       </c>

</xml_diff>

<commit_message>
New formula for calculating amplified temp sensor
</commit_message>
<xml_diff>
--- a/hardware/Verstaerker/Amplifier.xlsx
+++ b/hardware/Verstaerker/Amplifier.xlsx
@@ -30,9 +30,6 @@
     <t>ca. 20°C</t>
   </si>
   <si>
-    <t>(Messwert mit Sensor)</t>
-  </si>
-  <si>
     <t>(Gemessen mit Spannungsquelle anstelle des Sensors)</t>
   </si>
   <si>
@@ -55,6 +52,9 @@
   </si>
   <si>
     <t xml:space="preserve"> (909mV offset)</t>
+  </si>
+  <si>
+    <t>Formel (Ua*-0,485)+3,1</t>
   </si>
 </sst>
 </file>
@@ -377,81 +377,48 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="3"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$D$4</c:f>
+              <c:f>Tabelle1!$H$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ua</c:v>
+                  <c:v>Formel (Ua*-0,485)+3,1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Tabelle1!$B$5:$B$12</c:f>
-              <c:numCache>
-                <c:formatCode>0.000\ "V"</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0.90300000000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.1080000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.004</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.401</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.603</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.8009999999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$E$5:$E$12</c:f>
+              <c:f>Tabelle1!$I$5:$I$12</c:f>
               <c:numCache>
                 <c:formatCode>0\ "mV"</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>4483</c:v>
+                  <c:v>925.74499999999989</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4054.9999999999995</c:v>
+                  <c:v>1133.3250000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4234</c:v>
+                  <c:v>1046.5100000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3824</c:v>
+                  <c:v>1245.3600000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3400</c:v>
+                  <c:v>1451</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2972</c:v>
+                  <c:v>1658.58</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2768</c:v>
+                  <c:v>1757.52</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2552</c:v>
+                  <c:v>1862.28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -468,11 +435,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="100412416"/>
-        <c:axId val="100414208"/>
+        <c:axId val="101002240"/>
+        <c:axId val="101004032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100412416"/>
+        <c:axId val="101002240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -482,7 +449,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100414208"/>
+        <c:crossAx val="101004032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -490,10 +457,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100414208"/>
+        <c:axId val="101004032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.8"/>
+          <c:min val="850"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -502,7 +469,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100412416"/>
+        <c:crossAx val="101002240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -513,10 +480,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.6236102362204724"/>
-          <c:y val="0.62905365995917184"/>
+          <c:x val="0.60138801399825026"/>
+          <c:y val="0.43799660713142574"/>
           <c:w val="0.33750087489063868"/>
-          <c:h val="0.25115157480314959"/>
+          <c:h val="0.36787593623967735"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -558,7 +525,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$C$17</c:f>
+              <c:f>Tabelle1!$C$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -572,7 +539,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$B$18:$B$38</c:f>
+              <c:f>Tabelle1!$B$20:$B$40</c:f>
               <c:numCache>
                 <c:formatCode>0\ "mV"</c:formatCode>
                 <c:ptCount val="21"/>
@@ -644,7 +611,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$C$18:$C$33</c:f>
+              <c:f>Tabelle1!$C$20:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>0.00\ "°C"</c:formatCode>
                 <c:ptCount val="16"/>
@@ -706,7 +673,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$D$17</c:f>
+              <c:f>Tabelle1!$D$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -720,7 +687,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$B$18:$B$38</c:f>
+              <c:f>Tabelle1!$B$20:$B$40</c:f>
               <c:numCache>
                 <c:formatCode>0\ "mV"</c:formatCode>
                 <c:ptCount val="21"/>
@@ -792,7 +759,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$D$18:$D$33</c:f>
+              <c:f>Tabelle1!$D$20:$D$35</c:f>
               <c:numCache>
                 <c:formatCode>0.00\ "°C"</c:formatCode>
                 <c:ptCount val="16"/>
@@ -859,11 +826,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="100448128"/>
-        <c:axId val="100449664"/>
+        <c:axId val="101042048"/>
+        <c:axId val="101043584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100448128"/>
+        <c:axId val="101042048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -873,7 +840,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100449664"/>
+        <c:crossAx val="101043584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -881,7 +848,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100449664"/>
+        <c:axId val="101043584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -892,7 +859,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100448128"/>
+        <c:crossAx val="101042048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -926,7 +893,7 @@
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -950,13 +917,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>309561</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>185736</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>161924</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1266,10 +1233,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1277,39 +1244,41 @@
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
         <v>0.90300000000000002</v>
       </c>
@@ -1332,8 +1301,16 @@
         <f>(E5*-0.5)+3150</f>
         <v>908.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H5" s="2">
+        <f>(D5*-0.485)+3.1</f>
+        <v>0.92574500000000048</v>
+      </c>
+      <c r="I5" s="9">
+        <f>(E5*-0.485)+3100</f>
+        <v>925.74499999999989</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -1359,11 +1336,16 @@
         <f t="shared" ref="G6:G12" si="2">(E6*-0.5)+3150</f>
         <v>1122.5000000000002</v>
       </c>
-      <c r="H6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H6" s="2">
+        <f t="shared" ref="H6:H12" si="3">(D6*-0.485)+3.1</f>
+        <v>1.1333250000000004</v>
+      </c>
+      <c r="I6" s="9">
+        <f t="shared" ref="I6:I12" si="4">(E6*-0.485)+3100</f>
+        <v>1133.3250000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
         <v>1.004</v>
       </c>
@@ -1386,8 +1368,16 @@
         <f t="shared" si="2"/>
         <v>1033</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7" s="2">
+        <f t="shared" si="3"/>
+        <v>1.0465100000000001</v>
+      </c>
+      <c r="I7" s="9">
+        <f t="shared" si="4"/>
+        <v>1046.5100000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
         <v>1.2</v>
       </c>
@@ -1410,8 +1400,16 @@
         <f t="shared" si="2"/>
         <v>1238</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H8" s="2">
+        <f t="shared" si="3"/>
+        <v>1.2453600000000002</v>
+      </c>
+      <c r="I8" s="9">
+        <f t="shared" si="4"/>
+        <v>1245.3600000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>1.401</v>
       </c>
@@ -1434,8 +1432,16 @@
         <f t="shared" si="2"/>
         <v>1450</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" s="2">
+        <f t="shared" si="3"/>
+        <v>1.4510000000000001</v>
+      </c>
+      <c r="I9" s="9">
+        <f t="shared" si="4"/>
+        <v>1451</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>1.603</v>
       </c>
@@ -1458,8 +1464,16 @@
         <f t="shared" si="2"/>
         <v>1664</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H10" s="2">
+        <f t="shared" si="3"/>
+        <v>1.6585800000000002</v>
+      </c>
+      <c r="I10" s="9">
+        <f t="shared" si="4"/>
+        <v>1658.58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
         <v>1.7</v>
       </c>
@@ -1482,8 +1496,16 @@
         <f t="shared" si="2"/>
         <v>1766</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" s="2">
+        <f t="shared" si="3"/>
+        <v>1.7575200000000002</v>
+      </c>
+      <c r="I11" s="9">
+        <f t="shared" si="4"/>
+        <v>1757.52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
         <v>1.8009999999999999</v>
       </c>
@@ -1506,333 +1528,341 @@
         <f t="shared" si="2"/>
         <v>1874</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="H12" s="2">
+        <f t="shared" si="3"/>
+        <v>1.8622800000000002</v>
+      </c>
+      <c r="I12" s="9">
+        <f t="shared" si="4"/>
+        <v>1862.28</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>1</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
         <v>9</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E19" t="s">
         <v>10</v>
-      </c>
-      <c r="E17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="9">
-        <v>850</v>
-      </c>
-      <c r="C18" s="10">
-        <v>-3.41</v>
-      </c>
-      <c r="D18" s="10">
-        <v>-4.2</v>
-      </c>
-      <c r="E18" s="11">
-        <f>C18-D18</f>
-        <v>0.79</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="9">
-        <v>860</v>
-      </c>
-      <c r="C19" s="10">
-        <v>-2.4300000000000002</v>
-      </c>
-      <c r="D19" s="10">
-        <v>-3.3</v>
-      </c>
-      <c r="E19" s="11">
-        <f t="shared" ref="E19:E38" si="3">C19-D19</f>
-        <v>0.86999999999999966</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="9">
-        <v>870</v>
+        <v>850</v>
       </c>
       <c r="C20" s="10">
-        <v>-1.45</v>
+        <v>-3.41</v>
       </c>
       <c r="D20" s="10">
-        <v>-2.2000000000000002</v>
+        <v>-4.2</v>
       </c>
       <c r="E20" s="11">
-        <f t="shared" si="3"/>
-        <v>0.75000000000000022</v>
+        <f>C20-D20</f>
+        <v>0.79</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="9">
-        <v>880</v>
+        <v>860</v>
       </c>
       <c r="C21" s="10">
-        <v>-0.35</v>
+        <v>-2.4300000000000002</v>
       </c>
       <c r="D21" s="10">
-        <v>-1.3</v>
+        <v>-3.3</v>
       </c>
       <c r="E21" s="11">
-        <f t="shared" si="3"/>
-        <v>0.95000000000000007</v>
+        <f t="shared" ref="E21:E40" si="5">C21-D21</f>
+        <v>0.86999999999999966</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="9">
-        <v>890</v>
+        <v>870</v>
       </c>
       <c r="C22" s="10">
-        <v>0.5</v>
+        <v>-1.45</v>
       </c>
       <c r="D22" s="10">
-        <v>-0.33</v>
+        <v>-2.2000000000000002</v>
       </c>
       <c r="E22" s="11">
-        <f t="shared" si="3"/>
-        <v>0.83000000000000007</v>
+        <f t="shared" si="5"/>
+        <v>0.75000000000000022</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="9">
-        <v>900</v>
+        <v>880</v>
       </c>
       <c r="C23" s="10">
-        <v>1.48</v>
+        <v>-0.35</v>
       </c>
       <c r="D23" s="10">
-        <v>0.6</v>
+        <v>-1.3</v>
       </c>
       <c r="E23" s="11">
-        <f t="shared" si="3"/>
-        <v>0.88</v>
+        <f t="shared" si="5"/>
+        <v>0.95000000000000007</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="9">
-        <v>910</v>
+        <v>890</v>
       </c>
       <c r="C24" s="10">
-        <v>2.58</v>
+        <v>0.5</v>
       </c>
       <c r="D24" s="10">
-        <v>1.75</v>
+        <v>-0.33</v>
       </c>
       <c r="E24" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.83000000000000007</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="9">
-        <v>920</v>
+        <v>900</v>
       </c>
       <c r="C25" s="10">
-        <v>3.55</v>
+        <v>1.48</v>
       </c>
       <c r="D25" s="10">
-        <v>2.91</v>
+        <v>0.6</v>
       </c>
       <c r="E25" s="11">
-        <f t="shared" si="3"/>
-        <v>0.63999999999999968</v>
+        <f t="shared" si="5"/>
+        <v>0.88</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="9">
-        <v>930</v>
+        <v>910</v>
       </c>
       <c r="C26" s="10">
-        <v>4.54</v>
+        <v>2.58</v>
       </c>
       <c r="D26" s="10">
-        <v>3.7</v>
+        <v>1.75</v>
       </c>
       <c r="E26" s="11">
-        <f t="shared" si="3"/>
-        <v>0.83999999999999986</v>
+        <f t="shared" si="5"/>
+        <v>0.83000000000000007</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="9">
-        <v>940</v>
+        <v>920</v>
       </c>
       <c r="C27" s="10">
-        <v>5.5</v>
+        <v>3.55</v>
       </c>
       <c r="D27" s="10">
-        <v>4.8</v>
+        <v>2.91</v>
       </c>
       <c r="E27" s="11">
-        <f t="shared" si="3"/>
-        <v>0.70000000000000018</v>
+        <f t="shared" si="5"/>
+        <v>0.63999999999999968</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="9">
-        <v>950</v>
+        <v>930</v>
       </c>
       <c r="C28" s="10">
-        <v>6.6</v>
+        <v>4.54</v>
       </c>
       <c r="D28" s="10">
-        <v>5.78</v>
+        <v>3.7</v>
       </c>
       <c r="E28" s="11">
-        <f t="shared" si="3"/>
-        <v>0.8199999999999994</v>
+        <f t="shared" si="5"/>
+        <v>0.83999999999999986</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="9">
-        <v>960</v>
+        <v>940</v>
       </c>
       <c r="C29" s="10">
-        <v>7.58</v>
+        <v>5.5</v>
       </c>
       <c r="D29" s="10">
-        <v>6.81</v>
+        <v>4.8</v>
       </c>
       <c r="E29" s="11">
-        <f t="shared" si="3"/>
-        <v>0.77000000000000046</v>
+        <f t="shared" si="5"/>
+        <v>0.70000000000000018</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="9">
-        <v>970</v>
+        <v>950</v>
       </c>
       <c r="C30" s="10">
-        <v>8.56</v>
+        <v>6.6</v>
       </c>
       <c r="D30" s="10">
-        <v>7.91</v>
+        <v>5.78</v>
       </c>
       <c r="E30" s="11">
-        <f t="shared" si="3"/>
-        <v>0.65000000000000036</v>
+        <f t="shared" si="5"/>
+        <v>0.8199999999999994</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="9">
-        <v>980</v>
+        <v>960</v>
       </c>
       <c r="C31" s="10">
-        <v>9.5299999999999994</v>
+        <v>7.58</v>
       </c>
       <c r="D31" s="10">
-        <v>8.9499999999999993</v>
+        <v>6.81</v>
       </c>
       <c r="E31" s="11">
-        <f t="shared" si="3"/>
-        <v>0.58000000000000007</v>
+        <f t="shared" si="5"/>
+        <v>0.77000000000000046</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="9">
-        <v>990</v>
+        <v>970</v>
       </c>
       <c r="C32" s="10">
-        <v>10.51</v>
+        <v>8.56</v>
       </c>
       <c r="D32" s="10">
-        <v>10.17</v>
+        <v>7.91</v>
       </c>
       <c r="E32" s="11">
-        <f t="shared" si="3"/>
-        <v>0.33999999999999986</v>
+        <f t="shared" si="5"/>
+        <v>0.65000000000000036</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="9">
-        <v>1000</v>
+        <v>980</v>
       </c>
       <c r="C33" s="10">
-        <v>11.98</v>
+        <v>9.5299999999999994</v>
       </c>
       <c r="D33" s="10">
-        <v>11.33</v>
+        <v>8.9499999999999993</v>
       </c>
       <c r="E33" s="11">
-        <f t="shared" si="3"/>
-        <v>0.65000000000000036</v>
+        <f t="shared" si="5"/>
+        <v>0.58000000000000007</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="9">
-        <v>1100</v>
+        <v>990</v>
       </c>
       <c r="C34" s="10">
-        <v>21.86</v>
+        <v>10.51</v>
       </c>
       <c r="D34" s="10">
-        <v>21.89</v>
+        <v>10.17</v>
       </c>
       <c r="E34" s="11">
-        <f t="shared" si="3"/>
-        <v>-3.0000000000001137E-2</v>
+        <f t="shared" si="5"/>
+        <v>0.33999999999999986</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="9">
-        <v>1200</v>
+        <v>1000</v>
       </c>
       <c r="C35" s="10">
-        <v>32.119999999999997</v>
+        <v>11.98</v>
       </c>
       <c r="D35" s="10">
-        <v>32.200000000000003</v>
+        <v>11.33</v>
       </c>
       <c r="E35" s="11">
-        <f t="shared" si="3"/>
-        <v>-8.00000000000054E-2</v>
+        <f t="shared" si="5"/>
+        <v>0.65000000000000036</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="9">
-        <v>1300</v>
+        <v>1100</v>
       </c>
       <c r="C36" s="10">
-        <v>42</v>
+        <v>21.86</v>
       </c>
       <c r="D36" s="10">
-        <v>42.8</v>
+        <v>21.89</v>
       </c>
       <c r="E36" s="11">
-        <f t="shared" si="3"/>
-        <v>-0.79999999999999716</v>
+        <f t="shared" si="5"/>
+        <v>-3.0000000000001137E-2</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="9">
-        <v>1400</v>
+        <v>1200</v>
       </c>
       <c r="C37" s="10">
-        <v>52.89</v>
+        <v>32.119999999999997</v>
       </c>
       <c r="D37" s="10">
-        <v>52.9</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="E37" s="11">
-        <f t="shared" si="3"/>
-        <v>-9.9999999999980105E-3</v>
+        <f t="shared" si="5"/>
+        <v>-8.00000000000054E-2</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="9">
+        <v>1300</v>
+      </c>
+      <c r="C38" s="10">
+        <v>42</v>
+      </c>
+      <c r="D38" s="10">
+        <v>42.8</v>
+      </c>
+      <c r="E38" s="11">
+        <f t="shared" si="5"/>
+        <v>-0.79999999999999716</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="9">
+        <v>1400</v>
+      </c>
+      <c r="C39" s="10">
+        <v>52.89</v>
+      </c>
+      <c r="D39" s="10">
+        <v>52.9</v>
+      </c>
+      <c r="E39" s="11">
+        <f t="shared" si="5"/>
+        <v>-9.9999999999980105E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="9">
         <v>1500</v>
       </c>
-      <c r="C38" s="10">
+      <c r="C40" s="10">
         <v>62.15</v>
       </c>
-      <c r="D38" s="10">
+      <c r="D40" s="10">
         <v>64.13</v>
       </c>
-      <c r="E38" s="11">
-        <f t="shared" si="3"/>
+      <c r="E40" s="11">
+        <f t="shared" si="5"/>
         <v>-1.9799999999999969</v>
       </c>
     </row>

</xml_diff>